<commit_message>
Updated data and info
</commit_message>
<xml_diff>
--- a/data/tmb_fc_data.xlsx
+++ b/data/tmb_fc_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\imran\Desktop\Personal Projects\tmbfc-streamlit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866E38E7-18B4-4DE0-A3F0-AFB4A39087D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8471E6F-3540-468D-9084-90F114274E79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{E7419F15-B3CB-4403-AE17-0FD1F8C06D0E}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="69">
   <si>
     <t>player_name</t>
   </si>
@@ -153,6 +153,99 @@
   </si>
   <si>
     <t>Manchester United</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>player_rating</t>
+  </si>
+  <si>
+    <t>comparison_to_real_players</t>
+  </si>
+  <si>
+    <t>A midfielder with a forward's flair, Khalis is known for his rocket shots and feet that move faster than a squirrel on espresso.</t>
+  </si>
+  <si>
+    <t>The calm and collected Faris is a technical wizard in defense, with long balls that could reach the moon and back.</t>
+  </si>
+  <si>
+    <t>Virgil van Dijk, Toni Kroos</t>
+  </si>
+  <si>
+    <t>Hafiz is the reliable goal machine—he scores goals like it’s his job (because it is), and his defensive work rate is top-notch too!</t>
+  </si>
+  <si>
+    <t>Roberto Firmino, N'Golo Kanté</t>
+  </si>
+  <si>
+    <t>Defensive-minded and as strong as an ox, Danish also doubles as a goalkeeper when needed—talk about versatility!</t>
+  </si>
+  <si>
+    <t>John Terry, Peter Schmeichel</t>
+  </si>
+  <si>
+    <t>With flair, speed, and the ability to win headers like a giant, Imran is the forward that defenders dread facing.</t>
+  </si>
+  <si>
+    <t>Isa's stamina could put an Energizer Bunny to shame, and his strength makes him a brick wall on the field.</t>
+  </si>
+  <si>
+    <t>Kyle Walker, N’Golo Kanté</t>
+  </si>
+  <si>
+    <t>Muk is clinical in front of goal and technical with his feet, making him the kind of forward every team dreams of having.</t>
+  </si>
+  <si>
+    <t>Harry Kane, Riyad Mahrez</t>
+  </si>
+  <si>
+    <t>Abdullah’s technical skills and calm demeanor in goal make him the goalkeeper who could stay cool even in a snowstorm.</t>
+  </si>
+  <si>
+    <t>Ederson, Xabi Alonso</t>
+  </si>
+  <si>
+    <t>Farhan is a shot-stopper extraordinaire—he saves shots like he's got a magnetic glove.</t>
+  </si>
+  <si>
+    <t>Jan Oblak, Keylor Navas</t>
+  </si>
+  <si>
+    <t>Ashraf is a defensive powerhouse, strong enough to stop aerial threats and still have time to grab a snack.</t>
+  </si>
+  <si>
+    <t>Sergio Ramos, Giorgio Chiellini</t>
+  </si>
+  <si>
+    <t>Hamizan's positioning is so good, he could find the perfect spot in a crowded room, and his passing is like a GPS system for his teammates.</t>
+  </si>
+  <si>
+    <t>Thomas Müller, David Silva</t>
+  </si>
+  <si>
+    <t>With his technical skills and speed, Hanif plays with flair that makes defenders look like they're stuck in quicksand.</t>
+  </si>
+  <si>
+    <t>Eden Hazard, Raheem Sterling</t>
+  </si>
+  <si>
+    <t>Nabil is a defensive rock, strong and dominant, and he’s the type of player who makes attackers rethink their life choices.</t>
+  </si>
+  <si>
+    <t>Mats Hummels, Virgil van Dijk</t>
+  </si>
+  <si>
+    <t>Gan is the workhorse of the team—strong, hardworking, and always ready to put in the extra effort, even if it means running through a wall.</t>
+  </si>
+  <si>
+    <t>James Milner, Claude Makélélé</t>
+  </si>
+  <si>
+    <t>Kevin De Bruyne, Heung Min Son</t>
+  </si>
+  <si>
+    <t>Kai Havertz, Cristiano Ronaldo</t>
   </si>
 </sst>
 </file>
@@ -558,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22DE7E2C-5480-4F0C-93D0-534FDAD46C67}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -569,11 +662,15 @@
     <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="112.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -592,8 +689,17 @@
       <c r="F1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -612,8 +718,17 @@
       <c r="F2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2">
+        <v>88</v>
+      </c>
+      <c r="H2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -632,8 +747,17 @@
       <c r="F3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3">
+        <v>90</v>
+      </c>
+      <c r="H3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -652,8 +776,17 @@
       <c r="F4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4">
+        <v>81</v>
+      </c>
+      <c r="H4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -672,8 +805,17 @@
       <c r="F5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5">
+        <v>83</v>
+      </c>
+      <c r="H5" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -689,8 +831,17 @@
       <c r="F6" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6">
+        <v>82</v>
+      </c>
+      <c r="H6" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -706,8 +857,17 @@
       <c r="F7" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7">
+        <v>79</v>
+      </c>
+      <c r="H7" t="s">
+        <v>49</v>
+      </c>
+      <c r="I7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -723,8 +883,17 @@
       <c r="F8" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8">
+        <v>85</v>
+      </c>
+      <c r="H8" t="s">
+        <v>51</v>
+      </c>
+      <c r="I8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -743,8 +912,17 @@
       <c r="F9" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <v>86</v>
+      </c>
+      <c r="H9" t="s">
+        <v>53</v>
+      </c>
+      <c r="I9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -760,8 +938,17 @@
       <c r="F10" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10">
+        <v>85</v>
+      </c>
+      <c r="H10" t="s">
+        <v>55</v>
+      </c>
+      <c r="I10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -777,8 +964,17 @@
       <c r="F11" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G11">
+        <v>81</v>
+      </c>
+      <c r="H11" t="s">
+        <v>57</v>
+      </c>
+      <c r="I11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -797,8 +993,17 @@
       <c r="F12" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G12">
+        <v>82</v>
+      </c>
+      <c r="H12" t="s">
+        <v>59</v>
+      </c>
+      <c r="I12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -817,8 +1022,17 @@
       <c r="F13" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G13">
+        <v>87</v>
+      </c>
+      <c r="H13" t="s">
+        <v>61</v>
+      </c>
+      <c r="I13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -834,8 +1048,17 @@
       <c r="F14" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G14">
+        <v>81</v>
+      </c>
+      <c r="H14" t="s">
+        <v>63</v>
+      </c>
+      <c r="I14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -853,6 +1076,15 @@
       </c>
       <c r="F15" t="s">
         <v>36</v>
+      </c>
+      <c r="G15">
+        <v>79</v>
+      </c>
+      <c r="H15" t="s">
+        <v>65</v>
+      </c>
+      <c r="I15" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1792,7 +2024,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>